<commit_message>
scraping news data, saving data in excel and sending email with data
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,174 +437,229 @@
           <t>신문사</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>썸네일</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>"용돈 적다" 추석날 아내 폭행한 60대 쓰러진 채 발견(종합)</t>
+          <t>“추석 이동 줄었더니…가정폭력·교통사고 줄었다”(종합)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://yna.kr/AKR20201002019651065?did=1195m</t>
+          <t>https://www.seoul.co.kr/news/newsView.php?id=20201004500093&amp;wlog_tag3=naver</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>연합뉴스</t>
+          <t>네이버뉴스</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F081%2F2020%2F10%2F04%2F3128560.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>文대통령, 추석연휴 민생치안현장 방문···경찰·소방관 격려</t>
+          <t>"이 시국에 장·차관 홍보하나"...복지부 추석 포스터 논란</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://www.joseilbo.com/news/news_read.php?uid=407457&amp;class=32&amp;grp=</t>
+          <t>https://biz.chosun.com/site/data/html_dir/2020/10/04/2020100400542.html?utm_source=naver&amp;utm_medium=original&amp;utm_campaign=biz</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>조세일보</t>
+          <t>네이버뉴스</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F366%2F2020%2F10%2F04%2F598214.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>추석 연휴 이후 코로나19 대유행 우려…산발적 집단감염 잇따라</t>
+          <t>추석선물 백화점서 역대 가장 많이 샀다…"비쌀수록 인기"(종합)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://www.kwnews.co.kr/nview.asp?aid=220100100000</t>
+          <t>http://yna.kr/AKR20201004029351030?did=1195m</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>강원일보</t>
+          <t>네이버뉴스</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F001%2F2020%2F10%2F04%2F11919710.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>추석 제주 관광객 20만 명…4일까지 30만 명 방문 예상</t>
+          <t>복지부, '장관 얼굴' 추석 포스터 논란에 "물의 일으켜 송구"</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://news.sbs.co.kr/news/endPage.do?news_id=N1006006389&amp;plink=ORI&amp;cooper=NAVER</t>
+          <t>http://www.busan.com/view/busan/view.php?code=2020100417233211300</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SBS</t>
+          <t>네이버뉴스</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F082%2F2020%2F10%2F04%2F1033079.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>'코로나 추석'…정은경이 꼽은 위험요소 '셋'</t>
+          <t>추석 연휴 이후에도 수도권 고위험시설 영업중단은 계속</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://news.khan.co.kr/kh_news/khan_art_view.html?artid=202010021718001&amp;code=940100</t>
+          <t>http://news.kmib.co.kr/article/view.asp?arcid=0015072804&amp;code=61121111&amp;cp=nv</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>경향신문</t>
+          <t>네이버뉴스</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F005%2F2020%2F10%2F04%2F1367473.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>수원시청 임태혁, 추석씨름에서 15번째 금강장사 등극</t>
+          <t>수월한 추석 귀경길…"고속도로, 평소 주말보다 원활"</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>http://news.kbs.co.kr/news/view.do?ncd=5016946&amp;ref=A</t>
+          <t>http://www.newsis.com/view/?id=NISX20201004_0001185650&amp;cID=10201&amp;pID=10200</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>KBS</t>
+          <t>네이버뉴스</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F003%2F2020%2F10%2F04%2F10106636.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>소시지 3개에 김치 3조각... 격리된 병사가 먹은 추석날 저녁</t>
+          <t>추석 나훈아 소신발언에…野 "속 시원하게 文 비판" 與 "오독 말라"</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>http://www.ohmynews.com/NWS_Web/View/at_pg.aspx?CNTN_CD=A0002680782&amp;CMPT_CD=P0010&amp;utm_source=naver&amp;utm_medium=newsearch&amp;utm_campaign=naver_news</t>
+          <t>http://news.mk.co.kr/newsRead.php?no=1012678&amp;year=2020</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>오마이뉴스</t>
+          <t>네이버뉴스</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F009%2F2020%2F10%2F04%2F4667218.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>추석 다음날 아침 귀경길 고속도로 원활…부산-서울 5시간10분</t>
+          <t>추석 전 못 받은 2차 재난지원금, 연휴 뒤 10~11월에 지급</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://cnbc.sbs.co.kr/article_hub/10000998149?division=NAVER</t>
+          <t>https://www.chosun.com/economy/2020/10/04/YTRRE6TK2FGEHI6TF2PDWEUGVE/?utm_source=naver&amp;utm_medium=original&amp;utm_campaign=news</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SBS</t>
+          <t>네이버뉴스</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F023%2F2020%2F10%2F04%2F3566076.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>추석 귀경길 정체 구간 늘어나…‘저녁 8~9시 해소 전망’</t>
+          <t>코로나19 신규확진 64명 추석 귀성·귀경객 2명 확진 판정</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>http://www.edaily.co.kr/news/newspath.asp?newsid=01594086625928984</t>
+          <t>http://www.dongascience.com/news/view/40274</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>이데일리</t>
+          <t>네이버뉴스</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F584%2F2020%2F10%2F04%2F10730.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>“고만해라, 언제까지 싸울끼고” 부산 추석상 메뉴는 또 신공항</t>
+          <t>'코로나19' 덮친 추석 연휴, 교통사고·112신고 줄었다</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.chosun.com/national/national_general/2020/10/03/QMCYSY26I5ELDBMSZSPGWEPF6M/?utm_source=naver&amp;utm_medium=original&amp;utm_campaign=news</t>
+          <t>https://www.nocutnews.co.kr/news/5422084</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>조선일보</t>
+          <t>네이버뉴스</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F079%2F2020%2F10%2F04%2F3413806.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>

</xml_diff>